<commit_message>
Rough Rough Draft Complete
Added in Outer Bound Models, numerical results including tables and a very small conclusion.
</commit_message>
<xml_diff>
--- a/CurrentCodeAndResults/Tables/AlternativeModels.xlsx
+++ b/CurrentCodeAndResults/Tables/AlternativeModels.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben Rapone\Documents\Research\OPF\OPF\CurrentCodeAndResults\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben Rapone\Documents\Research\OPF\OPF\CurrentCodeAndResults\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14250" yWindow="0" windowWidth="4680" windowHeight="8070" activeTab="4" xr2:uid="{1D9B299A-2711-48A8-B4C7-CFA685D09CD6}"/>
+    <workbookView xWindow="15675" yWindow="0" windowWidth="4680" windowHeight="8070" xr2:uid="{1D9B299A-2711-48A8-B4C7-CFA685D09CD6}"/>
   </bookViews>
   <sheets>
     <sheet name="ResultsTable" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>Case #</t>
   </si>
@@ -41,31 +41,10 @@
     <t>B</t>
   </si>
   <si>
-    <t>Crad</t>
-  </si>
-  <si>
     <t>Times</t>
   </si>
   <si>
-    <t xml:space="preserve">Inner MIP Bd Z Feasibility </t>
-  </si>
-  <si>
-    <t>Outer BD LP Minimum C</t>
-  </si>
-  <si>
-    <t>Gap</t>
-  </si>
-  <si>
     <t>NA</t>
-  </si>
-  <si>
-    <t>5 Variables Nodes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inner LP Feasibility </t>
-  </si>
-  <si>
-    <t>Inner Linear Relaxation Bound Tightening</t>
   </si>
   <si>
     <t>Robustness of Solutio nwith respect to Variability of DERs</t>
@@ -75,6 +54,33 @@
   </si>
   <si>
     <t>Computational Time for Robustness Models</t>
+  </si>
+  <si>
+    <t>Gap between Outer Bd</t>
+  </si>
+  <si>
+    <t>Max Robust Margin</t>
+  </si>
+  <si>
+    <t>Min Robust Margin</t>
+  </si>
+  <si>
+    <t>Computational Time</t>
+  </si>
+  <si>
+    <t>1st 5 Variable Nodes</t>
+  </si>
+  <si>
+    <t>LP Bound Tightening Model</t>
+  </si>
+  <si>
+    <t>MIP Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LP Feasibility </t>
+  </si>
+  <si>
+    <t>Outer Bound Model B</t>
   </si>
 </sst>
 </file>
@@ -165,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -177,9 +183,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -217,6 +220,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -704,7 +719,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -744,7 +759,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -10292,15 +10307,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF4E2A94-A81C-4B7C-A6E2-715C5DFC85CB}">
   <dimension ref="A1:X22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="8" width="14.42578125" style="3" customWidth="1"/>
-    <col min="9" max="13" width="14.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="10.28515625" style="1" customWidth="1"/>
+    <col min="3" max="8" width="15.85546875" style="3" customWidth="1"/>
+    <col min="9" max="11" width="15.85546875" style="1" customWidth="1"/>
+    <col min="12" max="13" width="14.42578125" style="1" customWidth="1"/>
     <col min="14" max="14" width="15" style="1" customWidth="1"/>
     <col min="15" max="15" width="17.140625" style="1" customWidth="1"/>
     <col min="16" max="16" width="16.140625" style="1" customWidth="1"/>
@@ -10310,119 +10327,119 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" s="17"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
+      <c r="A1" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="16"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:24" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="X2" s="2"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="X2" s="18"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>57</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>1E-3</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="6">
+      <c r="C3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="5">
         <v>3.1010001306600002E-3</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="8">
         <v>489224.36623300001</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="5">
         <f t="shared" ref="K3:K15" si="0">L3-I3</f>
         <v>3.0454030484039999E-2</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="5">
         <v>3.3555030614699999E-2</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="5">
         <v>45144.120746699999</v>
       </c>
       <c r="N3" s="2"/>
@@ -10432,46 +10449,46 @@
       <c r="W3" s="2"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
+      <c r="A4" s="10">
         <v>30</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="10">
         <v>1E-3</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <v>2.00099964897E-3</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <v>36217.801035800003</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="10">
         <f t="shared" ref="E4:E6" si="1">L4-C4</f>
         <v>6.2901935664899994E-3</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <v>1.4009996489699999E-3</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="11">
         <v>2890.11111867</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="10">
         <f>L4-F4</f>
         <v>6.8901935664899992E-3</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="10">
         <v>2.2009996489700001E-3</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="10">
         <v>16388.4375674</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4" s="12">
         <f t="shared" si="0"/>
         <v>6.0901935664899997E-3</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="10">
         <v>8.2911932154599993E-3</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="10">
         <v>1025.35924636</v>
       </c>
       <c r="N4" s="2"/>
@@ -10481,46 +10498,46 @@
       <c r="W4" s="2"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+      <c r="A5" s="10">
         <v>30</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>1.1300999649E-2</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <v>49811.453777000002</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="12">
         <f t="shared" si="1"/>
         <v>2.9332132496600001E-2</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <v>6.9009996489699998E-3</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="10">
         <v>31427.987924000001</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="10">
         <f t="shared" ref="H5:H6" si="2">L5-F5</f>
         <v>3.3732132496629999E-2</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="10">
         <v>1.0500999649E-2</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="11">
         <v>22736.120920199999</v>
       </c>
-      <c r="K5" s="15">
+      <c r="K5" s="14">
         <f t="shared" si="0"/>
         <v>3.01321324966E-2</v>
       </c>
-      <c r="L5" s="11">
+      <c r="L5" s="10">
         <v>4.06331321456E-2</v>
       </c>
-      <c r="M5" s="11">
+      <c r="M5" s="10">
         <v>1031.1840538900001</v>
       </c>
       <c r="N5" s="2"/>
@@ -10529,276 +10546,276 @@
       <c r="S5" s="4"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+      <c r="A6" s="10">
         <v>30</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="10">
         <v>0.01</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="10">
         <v>2.2800999648999998E-2</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="10">
         <v>81609.172476499996</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="12">
         <f t="shared" si="1"/>
         <v>5.6403114555500011E-2</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="10">
         <v>1.2800999649E-2</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="11">
         <v>35052.439887400003</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="10">
         <f t="shared" si="2"/>
         <v>6.6403114555500006E-2</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="10">
         <v>1.9001000000000001E-2</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="10">
         <v>37329.836349999998</v>
       </c>
-      <c r="K6" s="15">
+      <c r="K6" s="14">
         <f t="shared" si="0"/>
         <v>6.0203114204500002E-2</v>
       </c>
-      <c r="L6" s="11">
+      <c r="L6" s="10">
         <v>7.9204114204500006E-2</v>
       </c>
-      <c r="M6" s="11">
+      <c r="M6" s="10">
         <v>1026.7231675999999</v>
       </c>
       <c r="N6" s="2"/>
       <c r="Q6" s="2"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>14</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>1E-3</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>2.7009999999999998E-3</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>895.20268417600005</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <f t="shared" ref="E7:E8" si="3">L7-C7</f>
         <v>4.8236249562600003E-3</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <v>1.3010000000000001E-3</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="8">
         <v>54.848490409999997</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <f t="shared" ref="H7:H15" si="4">L7-F7</f>
         <v>6.2236249562599997E-3</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="5">
         <v>3.0010000000000002E-3</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="5">
         <v>252.53735784899999</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="9">
         <f t="shared" si="0"/>
         <v>4.5236249562599995E-3</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="5">
         <v>7.5246249562599997E-3</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="5">
         <v>55.452757829900001</v>
       </c>
       <c r="N7" s="2"/>
       <c r="Q7" s="2"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>14</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>1.4701000000000001E-2</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>1523.3429410000001</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <f t="shared" si="3"/>
         <v>2.2400235621700001E-2</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <v>6.6010000000000001E-3</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="8">
         <v>143.96881479999999</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <f t="shared" si="4"/>
         <v>3.0500235621700001E-2</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="5">
         <v>1.4701000000000001E-2</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="5">
         <v>711.89906566399998</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="9">
         <f t="shared" si="0"/>
         <v>2.2400235621700001E-2</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L8" s="5">
         <v>3.71012356217E-2</v>
       </c>
-      <c r="M8" s="6">
+      <c r="M8" s="5">
         <v>55.871053530700003</v>
       </c>
       <c r="N8" s="2"/>
       <c r="Q8" s="2"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>14</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>0.01</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>2.9801000000000001E-2</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>3585.7141704400001</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <f>L9-C9</f>
         <v>4.3392681172399993E-2</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <v>1.3001E-2</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="8">
         <v>61.562664269999999</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <f t="shared" si="4"/>
         <v>6.0192681172399995E-2</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="5">
         <v>2.8701000000000001E-2</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="5">
         <v>885.25705990799997</v>
       </c>
-      <c r="K9" s="10">
+      <c r="K9" s="9">
         <f t="shared" si="0"/>
         <v>4.4492681172399989E-2</v>
       </c>
-      <c r="L9" s="6">
+      <c r="L9" s="5">
         <v>7.3193681172399994E-2</v>
       </c>
-      <c r="M9" s="6">
+      <c r="M9" s="5">
         <v>55.0753618528</v>
       </c>
       <c r="N9" s="2"/>
       <c r="Q9" s="2"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
+      <c r="A10" s="10">
         <v>9</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="10">
         <v>1E-3</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="13">
         <v>3.2009999999999999E-3</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="10">
         <v>29.5252099044</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="10">
         <f t="shared" ref="E10:E11" si="5">L10-C10</f>
         <v>5.6541517516100004E-3</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="13">
         <v>3.5010000000000002E-3</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="11">
         <v>4.3753266057899998</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="12">
         <f t="shared" si="4"/>
         <v>5.3541517516099996E-3</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="10">
         <v>3.5010000000000002E-3</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="10">
         <v>5.5200258632699999</v>
       </c>
-      <c r="K10" s="13">
+      <c r="K10" s="12">
         <f t="shared" si="0"/>
         <v>5.3541517516099996E-3</v>
       </c>
-      <c r="L10" s="11">
+      <c r="L10" s="10">
         <v>8.8551517516100003E-3</v>
       </c>
-      <c r="M10" s="11">
+      <c r="M10" s="10">
         <v>4.9468695302999999</v>
       </c>
       <c r="N10" s="2"/>
       <c r="Q10" s="2"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
+      <c r="A11" s="10">
         <v>9</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="13">
         <v>1.7600999999999999E-2</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="10">
         <v>66.340857561000007</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="10">
         <f t="shared" si="5"/>
         <v>2.6855080451600004E-2</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="13">
         <v>1.7701000000000001E-2</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="11">
         <v>9.6630591429999999</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H11" s="12">
         <f t="shared" si="4"/>
         <v>2.6755080451600001E-2</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="10">
         <v>1.7701000000000001E-2</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="10">
         <v>10.168007369</v>
       </c>
-      <c r="K11" s="13">
+      <c r="K11" s="12">
         <f t="shared" si="0"/>
         <v>2.6755080451600001E-2</v>
       </c>
-      <c r="L11" s="11">
+      <c r="L11" s="10">
         <v>4.4456080451600002E-2</v>
       </c>
-      <c r="M11" s="11">
+      <c r="M11" s="10">
         <v>5.1847513589099998</v>
       </c>
       <c r="N11" s="2"/>
@@ -10806,46 +10823,46 @@
       <c r="W11" s="2"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
+      <c r="A12" s="10">
         <v>9</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="10">
         <v>0.01</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="13">
         <v>3.5601000000000001E-2</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="10">
         <v>69.584210625300003</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="12">
         <f>L12-C12</f>
         <v>5.3761731931699995E-2</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="13">
         <v>3.4800999999999999E-2</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="11">
         <v>8.5786530879999994</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="10">
         <f t="shared" si="4"/>
         <v>5.4561731931699997E-2</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="10">
         <v>3.4800999999999999E-2</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="10">
         <v>11.424956948</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="10">
         <f t="shared" si="0"/>
         <v>5.4561731931699997E-2</v>
       </c>
-      <c r="L12" s="11">
+      <c r="L12" s="10">
         <v>8.9362731931699996E-2</v>
       </c>
-      <c r="M12" s="11">
+      <c r="M12" s="10">
         <v>5.6794617462600003</v>
       </c>
       <c r="N12" s="2"/>
@@ -10853,46 +10870,46 @@
       <c r="W12" s="2"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>5</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>1E-3</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>1.9001000000000001E-2</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>6.0077979199999998</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <f t="shared" ref="E13:E14" si="6">L13-C13</f>
         <v>4.7521767502999995E-3</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <v>2.1400999989699999E-2</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="8">
         <v>0.37639611947399998</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="5">
         <f t="shared" si="4"/>
         <v>2.3521767606000006E-3</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="5">
         <v>2.1600999989700002E-2</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="5">
         <v>0.70882434568899999</v>
       </c>
-      <c r="K13" s="10">
+      <c r="K13" s="9">
         <f t="shared" si="0"/>
         <v>2.1521767605999984E-3</v>
       </c>
-      <c r="L13" s="6">
+      <c r="L13" s="5">
         <v>2.37531767503E-2</v>
       </c>
-      <c r="M13" s="6">
+      <c r="M13" s="5">
         <v>1.8223631797299999</v>
       </c>
       <c r="N13" s="2"/>
@@ -10900,46 +10917,46 @@
       <c r="W13" s="2"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="A14" s="5">
         <v>5</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>0.105001</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <v>18.328150260000001</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <f t="shared" si="6"/>
         <v>1.3783842306000008E-2</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="6">
         <v>0.10720099999</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="8">
         <v>1.0472651495900001</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="5">
         <f t="shared" si="4"/>
         <v>1.1583842316000001E-2</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14" s="5">
         <v>0.10750099999</v>
       </c>
-      <c r="J14" s="6">
+      <c r="J14" s="5">
         <v>1.85275851408</v>
       </c>
-      <c r="K14" s="10">
+      <c r="K14" s="9">
         <f t="shared" si="0"/>
         <v>1.1283842316000006E-2</v>
       </c>
-      <c r="L14" s="6">
+      <c r="L14" s="5">
         <v>0.118784842306</v>
       </c>
-      <c r="M14" s="6">
+      <c r="M14" s="5">
         <v>0.80845953154500005</v>
       </c>
       <c r="N14" s="2"/>
@@ -10947,46 +10964,46 @@
       <c r="W14" s="2"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="A15" s="5">
         <v>5</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <v>0.01</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>0.21100099999999999</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <v>20.654103330000002</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <f>L15-C15</f>
         <v>2.7260674217000014E-2</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="6">
         <v>0.21330099998999999</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="8">
         <v>1.62745216268</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="5">
         <f t="shared" si="4"/>
         <v>2.4960674227000018E-2</v>
       </c>
-      <c r="I15" s="6">
+      <c r="I15" s="5">
         <v>0.21350099999</v>
       </c>
-      <c r="J15" s="6">
+      <c r="J15" s="5">
         <v>2.5983627623599999</v>
       </c>
-      <c r="K15" s="10">
+      <c r="K15" s="9">
         <f t="shared" si="0"/>
         <v>2.4760674227000012E-2</v>
       </c>
-      <c r="L15" s="6">
+      <c r="L15" s="5">
         <v>0.23826167421700001</v>
       </c>
-      <c r="M15" s="6">
+      <c r="M15" s="5">
         <v>0.81425781425400001</v>
       </c>
       <c r="N15" s="2"/>
@@ -11065,18 +11082,18 @@
   <sheetData>
     <row r="1" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="M1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="M2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -11134,7 +11151,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>

</xml_diff>